<commit_message>
modyfing sterile hold boundaries
</commit_message>
<xml_diff>
--- a/valid_short_data.xlsx
+++ b/valid_short_data.xlsx
@@ -135,7 +135,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -181,10 +181,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -267,8 +263,8 @@
   </sheetPr>
   <dimension ref="A1:D538"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A323" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A505" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E534" activeCellId="0" sqref="E534"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5047,7 +5043,7 @@
         <v>117.22</v>
       </c>
       <c r="D341" s="3" t="n">
-        <v>114.43</v>
+        <v>121.01</v>
       </c>
     </row>
     <row r="342" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7689,10 +7685,10 @@
       <c r="B530" s="3" t="n">
         <v>122.81</v>
       </c>
-      <c r="C530" s="12" t="n">
+      <c r="C530" s="3" t="n">
         <v>122.47</v>
       </c>
-      <c r="D530" s="12" t="n">
+      <c r="D530" s="3" t="n">
         <v>122.98</v>
       </c>
     </row>
@@ -7703,10 +7699,10 @@
       <c r="B531" s="3" t="n">
         <v>122.71</v>
       </c>
-      <c r="C531" s="12" t="n">
-        <v>122.41</v>
-      </c>
-      <c r="D531" s="12" t="n">
+      <c r="C531" s="3" t="n">
+        <v>122.01</v>
+      </c>
+      <c r="D531" s="3" t="n">
         <v>122.97</v>
       </c>
     </row>
@@ -7715,12 +7711,12 @@
         <v>0.528819444444451</v>
       </c>
       <c r="B532" s="3" t="n">
-        <v>122.61</v>
-      </c>
-      <c r="C532" s="12" t="n">
-        <v>122.35</v>
-      </c>
-      <c r="D532" s="12" t="n">
+        <v>122.47</v>
+      </c>
+      <c r="C532" s="3" t="n">
+        <v>121.55</v>
+      </c>
+      <c r="D532" s="3" t="n">
         <v>122.96</v>
       </c>
     </row>
@@ -7729,12 +7725,12 @@
         <v>0.528877314814821</v>
       </c>
       <c r="B533" s="3" t="n">
-        <v>122.51</v>
-      </c>
-      <c r="C533" s="12" t="n">
-        <v>122.29</v>
-      </c>
-      <c r="D533" s="12" t="n">
+        <v>122.01</v>
+      </c>
+      <c r="C533" s="3" t="n">
+        <v>121.09</v>
+      </c>
+      <c r="D533" s="3" t="n">
         <v>122.95</v>
       </c>
     </row>
@@ -7743,12 +7739,12 @@
         <v>0.528935185185192</v>
       </c>
       <c r="B534" s="3" t="n">
-        <v>122.41</v>
-      </c>
-      <c r="C534" s="12" t="n">
-        <v>122.23</v>
-      </c>
-      <c r="D534" s="12" t="n">
+        <v>121.55</v>
+      </c>
+      <c r="C534" s="3" t="n">
+        <v>120.63</v>
+      </c>
+      <c r="D534" s="3" t="n">
         <v>122.94</v>
       </c>
     </row>
@@ -7757,12 +7753,12 @@
         <v>0.528993055555562</v>
       </c>
       <c r="B535" s="3" t="n">
-        <v>122.31</v>
-      </c>
-      <c r="C535" s="12" t="n">
-        <v>122.17</v>
-      </c>
-      <c r="D535" s="12" t="n">
+        <v>120.32</v>
+      </c>
+      <c r="C535" s="3" t="n">
+        <v>120.17</v>
+      </c>
+      <c r="D535" s="3" t="n">
         <v>122.93</v>
       </c>
     </row>
@@ -7771,13 +7767,13 @@
         <v>0.529050925925932</v>
       </c>
       <c r="B536" s="3" t="n">
-        <v>122.21</v>
-      </c>
-      <c r="C536" s="12" t="n">
-        <v>122.11</v>
-      </c>
-      <c r="D536" s="12" t="n">
-        <v>122.92</v>
+        <v>119.09</v>
+      </c>
+      <c r="C536" s="3" t="n">
+        <v>119.71</v>
+      </c>
+      <c r="D536" s="3" t="n">
+        <v>120.98</v>
       </c>
     </row>
     <row r="537" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7785,13 +7781,13 @@
         <v>0.529108796296303</v>
       </c>
       <c r="B537" s="3" t="n">
-        <v>122.11</v>
-      </c>
-      <c r="C537" s="12" t="n">
-        <v>122.05</v>
-      </c>
-      <c r="D537" s="12" t="n">
-        <v>122.91</v>
+        <v>117.86</v>
+      </c>
+      <c r="C537" s="3" t="n">
+        <v>119.25</v>
+      </c>
+      <c r="D537" s="3" t="n">
+        <v>120.81</v>
       </c>
     </row>
     <row r="538" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7799,13 +7795,13 @@
         <v>0.529166666666673</v>
       </c>
       <c r="B538" s="3" t="n">
-        <v>122.01</v>
-      </c>
-      <c r="C538" s="12" t="n">
-        <v>121.99</v>
-      </c>
-      <c r="D538" s="12" t="n">
-        <v>122.9</v>
+        <v>116.63</v>
+      </c>
+      <c r="C538" s="3" t="n">
+        <v>118.79</v>
+      </c>
+      <c r="D538" s="3" t="n">
+        <v>120.62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>